<commit_message>
Updated layout XLSX again
</commit_message>
<xml_diff>
--- a/sql/enrolment/LAYOUT_counts-of-status-and-priority.xlsx
+++ b/sql/enrolment/LAYOUT_counts-of-status-and-priority.xlsx
@@ -4,38 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>01 - Application Cancelled</t>
-  </si>
-  <si>
-    <t>02 - Alumni</t>
-  </si>
-  <si>
-    <t>03 - Past Enrolment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>04 - Returning Enrolment</t>
   </si>
   <si>
-    <t>05 - Current Enrolment</t>
-  </si>
-  <si>
-    <t>06 - Place Accepted</t>
-  </si>
-  <si>
     <t>07 - Offered Place</t>
   </si>
   <si>
@@ -54,15 +37,6 @@
     <t>13 - Interview Complete</t>
   </si>
   <si>
-    <t>12 - Enquiry</t>
-  </si>
-  <si>
-    <t>14 - Expired Offer</t>
-  </si>
-  <si>
-    <t>15 - Expired Application</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -91,13 +65,46 @@
   </si>
   <si>
     <t>06 - Other</t>
+  </si>
+  <si>
+    <t>SAMPLE DATA</t>
+  </si>
+  <si>
+    <t>Benjamin Ramos</t>
+  </si>
+  <si>
+    <t>Aaron King</t>
+  </si>
+  <si>
+    <t>Ernest Dunn</t>
+  </si>
+  <si>
+    <t>Wayne Ferguson</t>
+  </si>
+  <si>
+    <t>Sean Day</t>
+  </si>
+  <si>
+    <t>Raymond Cook</t>
+  </si>
+  <si>
+    <t>Charles Wallace</t>
+  </si>
+  <si>
+    <t>Stephen Moreno</t>
+  </si>
+  <si>
+    <t>Gary Scott</t>
+  </si>
+  <si>
+    <t>Willie Hernandez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +132,65 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF003300"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF003300"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF003366"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF003366"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF003366"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Monaco"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Monaco"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -163,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -211,19 +270,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color indexed="64"/>
       </left>
@@ -251,13 +297,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color theme="6" tint="-0.499984740745262"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -266,19 +312,21 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color theme="3" tint="-0.24994659260841701"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -337,14 +385,14 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color theme="4" tint="-0.499984740745262"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thick">
-        <color theme="3" tint="-0.24994659260841701"/>
+        <color theme="6" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -352,65 +400,141 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE8E8E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF003300"/>
+      <color rgb="FF003366"/>
+      <color rgb="FFE8E8E8"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
@@ -710,293 +834,513 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="18" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="16"/>
-    </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:16" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
   </sheetData>
+  <sortState ref="A13:C22">
+    <sortCondition ref="C13:C22"/>
+    <sortCondition ref="B13:B22"/>
+    <sortCondition ref="A13:A22"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B1:P1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B3:H10">
+    <cfRule type="notContainsText" dxfId="1" priority="1" operator="notContains" text="0">
+      <formula>ISERROR(SEARCH("0",B3))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="0">
+      <formula>NOT(ISERROR(SEARCH("0",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="120" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>